<commit_message>
Calibrate model with Roseires geometry data
</commit_message>
<xml_diff>
--- a/cases/gerd_roseires/input_data/roseires_geometry.xlsx
+++ b/cases/gerd_roseires/input_data/roseires_geometry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cvemo\Documents\my_stuff\Publication\flood-wave-propagation\cases\gerd_roseires\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D45B6A-564E-4A75-896B-084CA9B5E3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8232D534-A3A9-41A4-ABB0-7B3D65E40ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Stage</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Surface area</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>m^3</t>
   </si>
 </sst>
 </file>
@@ -83,13 +89,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -371,151 +380,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>467</v>
       </c>
       <c r="B3" s="1">
         <v>10500000</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="1">
+        <v>23.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>468</v>
       </c>
       <c r="B4" s="1">
         <v>16800000</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="1">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>469</v>
       </c>
       <c r="B5" s="1">
         <v>26300000</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
+        <v>58.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>470</v>
       </c>
       <c r="B6" s="1">
         <v>43200000</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>472</v>
       </c>
       <c r="B7" s="1">
         <v>93400000</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
+        <v>227.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>474</v>
       </c>
       <c r="B8" s="1">
         <v>144100000</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <v>472.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>476</v>
       </c>
       <c r="B9" s="1">
         <v>185200000</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>801.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>478</v>
       </c>
       <c r="B10" s="1">
         <v>225200000</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>480</v>
       </c>
       <c r="B11" s="1">
         <v>261300000</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>481</v>
       </c>
       <c r="B12" s="1">
         <v>280900000</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>482</v>
       </c>
       <c r="B13" s="1">
         <v>329500000</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <v>2282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>484</v>
       </c>
       <c r="B14" s="1">
         <v>389100000</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>486</v>
       </c>
       <c r="B15" s="1">
         <v>458800000</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>3847</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>488</v>
       </c>
       <c r="B16" s="1">
         <v>516600000</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>4824</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>490</v>
       </c>
       <c r="B17" s="1">
         <v>564500000</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5909</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>492</v>
+      </c>
+      <c r="B18" s="1">
+        <v>640191729</v>
+      </c>
+      <c r="C18" s="3">
+        <f>C17+(B17+B18)/1000000</f>
+        <v>7113.6917290000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>